<commit_message>
Add times for David and correct chip number duplication
</commit_message>
<xml_diff>
--- a/startlist.xlsx
+++ b/startlist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="255">
   <si>
     <t xml:space="preserve">Klass</t>
   </si>
@@ -551,6 +551,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bauhaus sportklubb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">??</t>
   </si>
   <si>
     <t xml:space="preserve">Mikael Germundsjö</t>
@@ -1079,11 +1082,11 @@
   </sheetPr>
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D84" activeCellId="0" sqref="D84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F56" activeCellId="0" sqref="F56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.79"/>
@@ -2184,10 +2187,10 @@
         <v>176</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>97</v>
+        <v>177</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2198,16 +2201,16 @@
         <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,16 +2221,16 @@
         <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2238,16 +2241,16 @@
         <v>56</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2258,16 +2261,16 @@
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2278,16 +2281,16 @@
         <v>58</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2298,16 +2301,16 @@
         <v>59</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,16 +2321,16 @@
         <v>60</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,16 +2341,16 @@
         <v>61</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,16 +2361,16 @@
         <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2378,16 +2381,16 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2398,16 +2401,16 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,16 +2421,16 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2438,16 +2441,16 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2458,16 +2461,16 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2478,16 +2481,16 @@
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2498,16 +2501,16 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,16 +2521,16 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2538,16 +2541,16 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2558,16 +2561,16 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2578,16 +2581,16 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,16 +2601,16 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>150</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2618,16 +2621,16 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,16 +2641,16 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,16 +2661,16 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2678,16 +2681,16 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2698,76 +2701,76 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B82" s="0" t="n">
+      <c r="B82" s="1" t="n">
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>172</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B83" s="0" t="n">
+      <c r="B83" s="1" t="n">
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>172</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B84" s="0" t="n">
+      <c r="A84" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B84" s="1" t="n">
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E84" s="0" t="s">
-        <v>253</v>
+      <c r="E84" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>